<commit_message>
Added exponential ratio, updated xlsx file
</commit_message>
<xml_diff>
--- a/lab_algo.xlsx
+++ b/lab_algo.xlsx
@@ -5,17 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaori/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaori/IdeaProjects/lab1_pestrikv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B81465B-8AD3-3D49-AE7B-F6BD948EF692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD054A9B-ECA4-FC49-9E76-8D9ECC911F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D4F34C4-6F3A-D647-AD59-3E2EE28ECA5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$21:$A$34</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$J$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$J$21:$J$34</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$A$20</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$A$21:$A$34</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$J$20</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$J$21:$J$34</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>M</t>
   </si>
@@ -48,6 +58,9 @@
   </si>
   <si>
     <t>EXP FIRST</t>
+  </si>
+  <si>
+    <t>EXP2/EXP1</t>
   </si>
 </sst>
 </file>
@@ -2699,6 +2712,384 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-KZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EXP2/EXP1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$21:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$21:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3.5529658382334656E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3112480739599383E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6009285151901828E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2136561771818792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80617386937239843</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39398546233354437</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1645016368322072</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9133003721074642E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23703502579418953</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.766583541147132E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4659803462798316E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8108716525702104</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93978129572967939</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65703791097382525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5A4-F04C-9D41-62278A9FBF64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="608220416"/>
+        <c:axId val="763595856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="608220416"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763595856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="763595856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-KZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="608220416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-KZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2779,6 +3170,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3296,6 +3727,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3880,6 +4827,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>665891</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>295189</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>204573</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F688152-31A7-B2B2-CC00-F5FDEAE5F5DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4185,10 +5168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF42ADF4-ED66-4146-82D9-75147D1EA78B}">
-  <dimension ref="A3:H34"/>
+  <dimension ref="A3:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4208,7 +5191,7 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -4224,8 +5207,11 @@
       <c r="H20" t="s">
         <v>3</v>
       </c>
+      <c r="J20" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -4241,8 +5227,12 @@
       <c r="H21">
         <v>2E-3</v>
       </c>
+      <c r="J21">
+        <f>(H21/D21)</f>
+        <v>3.5529658382334656E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -4258,8 +5248,12 @@
       <c r="H22">
         <v>1.8749999999999999E-3</v>
       </c>
+      <c r="J22">
+        <f t="shared" ref="J22:J34" si="0">(H22/D22)</f>
+        <v>2.3112480739599383E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4275,8 +5269,12 @@
       <c r="H23">
         <v>1.916E-3</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>2.6009285151901828E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>8</v>
       </c>
@@ -4292,8 +5290,12 @@
       <c r="H24">
         <v>0.57323000000000002</v>
       </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>4.2136561771818792</v>
+      </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>16</v>
       </c>
@@ -4309,8 +5311,12 @@
       <c r="H25">
         <v>0.189417</v>
       </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>0.80617386937239843</v>
+      </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>32</v>
       </c>
@@ -4326,8 +5332,12 @@
       <c r="H26">
         <v>0.23583299999999999</v>
       </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0.39398546233354437</v>
+      </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>64</v>
       </c>
@@ -4343,8 +5353,12 @@
       <c r="H27">
         <v>0.73562499999999997</v>
       </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>1.1645016368322072</v>
+      </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>128</v>
       </c>
@@ -4360,8 +5374,12 @@
       <c r="H28">
         <v>8.4292000000000006E-2</v>
       </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>9.9133003721074642E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>256</v>
       </c>
@@ -4377,8 +5395,12 @@
       <c r="H29">
         <v>0.109125</v>
       </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0.23703502579418953</v>
+      </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>512</v>
       </c>
@@ -4394,8 +5416,12 @@
       <c r="H30">
         <v>3.542E-3</v>
       </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>1.766583541147132E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1024</v>
       </c>
@@ -4411,8 +5437,12 @@
       <c r="H31">
         <v>3.9160000000000002E-3</v>
       </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>1.4659803462798316E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2048</v>
       </c>
@@ -4428,8 +5458,12 @@
       <c r="H32">
         <v>0.39416699999999999</v>
       </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>1.8108716525702104</v>
+      </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4096</v>
       </c>
@@ -4445,8 +5479,12 @@
       <c r="H33">
         <v>0.88304199999999999</v>
       </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>0.93978129572967939</v>
+      </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8192</v>
       </c>
@@ -4461,6 +5499,10 @@
       </c>
       <c r="H34">
         <v>1.9513750000000001</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>0.65703791097382525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now the tests are run 100 times and the average values are taken, this helped to correct errors in the indicators of the graphs.
</commit_message>
<xml_diff>
--- a/lab_algo.xlsx
+++ b/lab_algo.xlsx
@@ -8,23 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaori/IdeaProjects/lab1_pestrikv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD054A9B-ECA4-FC49-9E76-8D9ECC911F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47240599-0C41-C847-9DA4-DA0EE3823CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D4F34C4-6F3A-D647-AD59-3E2EE28ECA5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$21:$A$34</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$J$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$J$21:$J$34</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$A$20</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$A$21:$A$34</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$J$20</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$J$21:$J$34</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -246,9 +236,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -297,47 +284,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>5.2090000000000001E-3</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1669999999999997E-3</c:v>
+                  <c:v>23.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6660000000000001E-3</c:v>
+                  <c:v>134.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.156083</c:v>
+                  <c:v>298.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14908399999999999</c:v>
+                  <c:v>706.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25674999999999998</c:v>
+                  <c:v>1435.81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.121166</c:v>
+                  <c:v>3378.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47199999999999998</c:v>
+                  <c:v>7372.43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30287500000000001</c:v>
+                  <c:v>20446.16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9166999999999998E-2</c:v>
+                  <c:v>37361.300000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11600000000000001</c:v>
+                  <c:v>41112.11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39454099999999998</c:v>
+                  <c:v>51791.99</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1657090000000001</c:v>
+                  <c:v>104733.46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5979999999999999</c:v>
+                  <c:v>337165.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,9 +374,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -492,9 +473,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -543,47 +521,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>5.6291000000000001E-2</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1125000000000003E-2</c:v>
+                  <c:v>52.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3665999999999995E-2</c:v>
+                  <c:v>146.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.136041</c:v>
+                  <c:v>317.36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.234958</c:v>
+                  <c:v>702.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59858299999999998</c:v>
+                  <c:v>1533.23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63170800000000005</c:v>
+                  <c:v>3631.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85029200000000005</c:v>
+                  <c:v>8626.2199999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46037499999999998</c:v>
+                  <c:v>18368.57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.20050000000000001</c:v>
+                  <c:v>21572.13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.267125</c:v>
+                  <c:v>33467.32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.217667</c:v>
+                  <c:v>68421.039999999994</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.93962500000000004</c:v>
+                  <c:v>152643.62</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9699580000000001</c:v>
+                  <c:v>220632.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -636,9 +611,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -737,9 +709,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -788,47 +757,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.26083400000000001</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30266700000000002</c:v>
+                  <c:v>1418.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47112500000000002</c:v>
+                  <c:v>2124.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56354099999999996</c:v>
+                  <c:v>2883.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63295800000000002</c:v>
+                  <c:v>2531.6799999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72829100000000002</c:v>
+                  <c:v>2912.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98</c:v>
+                  <c:v>3267.42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62254100000000001</c:v>
+                  <c:v>4124.63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77391600000000005</c:v>
+                  <c:v>4497.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41470800000000002</c:v>
+                  <c:v>5731.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.28762500000000002</c:v>
+                  <c:v>12147.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32837499999999997</c:v>
+                  <c:v>22536.21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41212500000000002</c:v>
+                  <c:v>34864.21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.238791</c:v>
+                  <c:v>83174.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,9 +847,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -982,9 +945,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1033,47 +993,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2E-3</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8749999999999999E-3</c:v>
+                  <c:v>30.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.916E-3</c:v>
+                  <c:v>72.569999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57323000000000002</c:v>
+                  <c:v>146.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.189417</c:v>
+                  <c:v>294.20999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23583299999999999</c:v>
+                  <c:v>451.56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73562499999999997</c:v>
+                  <c:v>411.73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4292000000000006E-2</c:v>
+                  <c:v>733.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.109125</c:v>
+                  <c:v>1557.32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.542E-3</c:v>
+                  <c:v>2619.41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9160000000000002E-3</c:v>
+                  <c:v>4903.16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39416699999999999</c:v>
+                  <c:v>12542.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88304199999999999</c:v>
+                  <c:v>32513.63</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9513750000000001</c:v>
+                  <c:v>81572.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,7 +1056,6 @@
       <c:valAx>
         <c:axId val="1740788063"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1539,9 +1495,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1590,47 +1543,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>5.2090000000000001E-3</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1669999999999997E-3</c:v>
+                  <c:v>23.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6660000000000001E-3</c:v>
+                  <c:v>134.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.156083</c:v>
+                  <c:v>298.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14908399999999999</c:v>
+                  <c:v>706.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25674999999999998</c:v>
+                  <c:v>1435.81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.121166</c:v>
+                  <c:v>3378.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47199999999999998</c:v>
+                  <c:v>7372.43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30287500000000001</c:v>
+                  <c:v>20446.16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9166999999999998E-2</c:v>
+                  <c:v>37361.300000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11600000000000001</c:v>
+                  <c:v>41112.11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39454099999999998</c:v>
+                  <c:v>51791.99</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1657090000000001</c:v>
+                  <c:v>104733.46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5979999999999999</c:v>
+                  <c:v>337165.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1683,9 +1633,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1784,9 +1731,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1835,47 +1779,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>5.6291000000000001E-2</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1125000000000003E-2</c:v>
+                  <c:v>52.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3665999999999995E-2</c:v>
+                  <c:v>146.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.136041</c:v>
+                  <c:v>317.36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.234958</c:v>
+                  <c:v>702.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59858299999999998</c:v>
+                  <c:v>1533.23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63170800000000005</c:v>
+                  <c:v>3631.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85029200000000005</c:v>
+                  <c:v>8626.2199999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46037499999999998</c:v>
+                  <c:v>18368.57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.20050000000000001</c:v>
+                  <c:v>21572.13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.267125</c:v>
+                  <c:v>33467.32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.217667</c:v>
+                  <c:v>68421.039999999994</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.93962500000000004</c:v>
+                  <c:v>152643.62</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9699580000000001</c:v>
+                  <c:v>220632.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1928,9 +1869,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2031,9 +1969,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2082,47 +2017,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.26083400000000001</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30266700000000002</c:v>
+                  <c:v>1418.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47112500000000002</c:v>
+                  <c:v>2124.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56354099999999996</c:v>
+                  <c:v>2883.17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63295800000000002</c:v>
+                  <c:v>2531.6799999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72829100000000002</c:v>
+                  <c:v>2912.26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98</c:v>
+                  <c:v>3267.42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62254100000000001</c:v>
+                  <c:v>4124.63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77391600000000005</c:v>
+                  <c:v>4497.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41470800000000002</c:v>
+                  <c:v>5731.94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.28762500000000002</c:v>
+                  <c:v>12147.97</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32837499999999997</c:v>
+                  <c:v>22536.21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41212500000000002</c:v>
+                  <c:v>34864.21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.238791</c:v>
+                  <c:v>83174.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2175,9 +2107,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2276,9 +2205,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2327,47 +2253,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2E-3</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8749999999999999E-3</c:v>
+                  <c:v>30.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.916E-3</c:v>
+                  <c:v>72.569999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57323000000000002</c:v>
+                  <c:v>146.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.189417</c:v>
+                  <c:v>294.20999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23583299999999999</c:v>
+                  <c:v>451.56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73562499999999997</c:v>
+                  <c:v>411.73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4292000000000006E-2</c:v>
+                  <c:v>733.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.109125</c:v>
+                  <c:v>1557.32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.542E-3</c:v>
+                  <c:v>2619.41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9160000000000002E-3</c:v>
+                  <c:v>4903.16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39416699999999999</c:v>
+                  <c:v>12542.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88304199999999999</c:v>
+                  <c:v>32513.63</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9513750000000001</c:v>
+                  <c:v>81572.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2806,9 +2729,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2857,47 +2777,44 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>3.5529658382334656E-2</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3112480739599383E-2</c:v>
+                  <c:v>0.57789716039907912</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6009285151901828E-2</c:v>
+                  <c:v>0.49451448040885854</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2136561771818792</c:v>
+                  <c:v>0.46130577262414924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80617386937239843</c:v>
+                  <c:v>0.41862549800796811</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39398546233354437</c:v>
+                  <c:v>0.29451549995760584</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1645016368322072</c:v>
+                  <c:v>0.11337458248315477</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9133003721074642E-2</c:v>
+                  <c:v>8.5048839468504167E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23703502579418953</c:v>
+                  <c:v>8.4781776697913883E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.766583541147132E-2</c:v>
+                  <c:v>0.12142565430488318</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4659803462798316E-2</c:v>
+                  <c:v>0.14650590486480541</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8108716525702104</c:v>
+                  <c:v>0.18331641845841573</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.93978129572967939</c:v>
+                  <c:v>0.21300353070767059</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.65703791097382525</c:v>
+                  <c:v>0.36972195958062537</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5170,8 +5087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF42ADF4-ED66-4146-82D9-75147D1EA78B}">
   <dimension ref="A3:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5211,46 +5128,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>5.2090000000000001E-3</v>
-      </c>
-      <c r="D21">
-        <v>5.6291000000000001E-2</v>
-      </c>
-      <c r="F21">
-        <v>0.26083400000000001</v>
-      </c>
-      <c r="H21">
-        <v>2E-3</v>
-      </c>
-      <c r="J21">
-        <f>(H21/D21)</f>
-        <v>3.5529658382334656E-2</v>
-      </c>
-    </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2</v>
       </c>
       <c r="B22">
-        <v>6.1669999999999997E-3</v>
+        <v>23.54</v>
       </c>
       <c r="D22">
-        <v>8.1125000000000003E-2</v>
+        <v>52.12</v>
       </c>
       <c r="F22">
-        <v>0.30266700000000002</v>
+        <v>1418.24</v>
       </c>
       <c r="H22">
-        <v>1.8749999999999999E-3</v>
+        <v>30.12</v>
       </c>
       <c r="J22">
         <f t="shared" ref="J22:J34" si="0">(H22/D22)</f>
-        <v>2.3112480739599383E-2</v>
+        <v>0.57789716039907912</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -5258,20 +5154,20 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>7.6660000000000001E-3</v>
+        <v>134.35</v>
       </c>
       <c r="D23">
-        <v>7.3665999999999995E-2</v>
+        <v>146.75</v>
       </c>
       <c r="F23">
-        <v>0.47112500000000002</v>
+        <v>2124.1999999999998</v>
       </c>
       <c r="H23">
-        <v>1.916E-3</v>
+        <v>72.569999999999993</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>2.6009285151901828E-2</v>
+        <v>0.49451448040885854</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -5279,20 +5175,20 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>0.156083</v>
+        <v>298.14</v>
       </c>
       <c r="D24">
-        <v>0.136041</v>
+        <v>317.36</v>
       </c>
       <c r="F24">
-        <v>0.56354099999999996</v>
+        <v>2883.17</v>
       </c>
       <c r="H24">
-        <v>0.57323000000000002</v>
+        <v>146.4</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>4.2136561771818792</v>
+        <v>0.46130577262414924</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -5300,20 +5196,20 @@
         <v>16</v>
       </c>
       <c r="B25">
-        <v>0.14908399999999999</v>
+        <v>706.06</v>
       </c>
       <c r="D25">
-        <v>0.234958</v>
+        <v>702.8</v>
       </c>
       <c r="F25">
-        <v>0.63295800000000002</v>
+        <v>2531.6799999999998</v>
       </c>
       <c r="H25">
-        <v>0.189417</v>
+        <v>294.20999999999998</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>0.80617386937239843</v>
+        <v>0.41862549800796811</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -5321,20 +5217,20 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>0.25674999999999998</v>
+        <v>1435.81</v>
       </c>
       <c r="D26">
-        <v>0.59858299999999998</v>
+        <v>1533.23</v>
       </c>
       <c r="F26">
-        <v>0.72829100000000002</v>
+        <v>2912.26</v>
       </c>
       <c r="H26">
-        <v>0.23583299999999999</v>
+        <v>451.56</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.39398546233354437</v>
+        <v>0.29451549995760584</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -5342,20 +5238,20 @@
         <v>64</v>
       </c>
       <c r="B27">
-        <v>0.121166</v>
+        <v>3378.67</v>
       </c>
       <c r="D27">
-        <v>0.63170800000000005</v>
+        <v>3631.59</v>
       </c>
       <c r="F27">
-        <v>0.98</v>
+        <v>3267.42</v>
       </c>
       <c r="H27">
-        <v>0.73562499999999997</v>
+        <v>411.73</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>1.1645016368322072</v>
+        <v>0.11337458248315477</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -5363,20 +5259,20 @@
         <v>128</v>
       </c>
       <c r="B28">
-        <v>0.47199999999999998</v>
+        <v>7372.43</v>
       </c>
       <c r="D28">
-        <v>0.85029200000000005</v>
+        <v>8626.2199999999993</v>
       </c>
       <c r="F28">
-        <v>0.62254100000000001</v>
+        <v>4124.63</v>
       </c>
       <c r="H28">
-        <v>8.4292000000000006E-2</v>
+        <v>733.65</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>9.9133003721074642E-2</v>
+        <v>8.5048839468504167E-2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -5384,20 +5280,20 @@
         <v>256</v>
       </c>
       <c r="B29">
-        <v>0.30287500000000001</v>
+        <v>20446.16</v>
       </c>
       <c r="D29">
-        <v>0.46037499999999998</v>
+        <v>18368.57</v>
       </c>
       <c r="F29">
-        <v>0.77391600000000005</v>
+        <v>4497.5</v>
       </c>
       <c r="H29">
-        <v>0.109125</v>
+        <v>1557.32</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0.23703502579418953</v>
+        <v>8.4781776697913883E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -5405,20 +5301,20 @@
         <v>512</v>
       </c>
       <c r="B30">
-        <v>2.9166999999999998E-2</v>
+        <v>37361.300000000003</v>
       </c>
       <c r="D30">
-        <v>0.20050000000000001</v>
+        <v>21572.13</v>
       </c>
       <c r="F30">
-        <v>0.41470800000000002</v>
+        <v>5731.94</v>
       </c>
       <c r="H30">
-        <v>3.542E-3</v>
+        <v>2619.41</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>1.766583541147132E-2</v>
+        <v>0.12142565430488318</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -5426,20 +5322,20 @@
         <v>1024</v>
       </c>
       <c r="B31">
-        <v>0.11600000000000001</v>
+        <v>41112.11</v>
       </c>
       <c r="D31">
-        <v>0.267125</v>
+        <v>33467.32</v>
       </c>
       <c r="F31">
-        <v>0.28762500000000002</v>
+        <v>12147.97</v>
       </c>
       <c r="H31">
-        <v>3.9160000000000002E-3</v>
+        <v>4903.16</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>1.4659803462798316E-2</v>
+        <v>0.14650590486480541</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -5447,20 +5343,20 @@
         <v>2048</v>
       </c>
       <c r="B32">
-        <v>0.39454099999999998</v>
+        <v>51791.99</v>
       </c>
       <c r="D32">
-        <v>0.217667</v>
+        <v>68421.039999999994</v>
       </c>
       <c r="F32">
-        <v>0.32837499999999997</v>
+        <v>22536.21</v>
       </c>
       <c r="H32">
-        <v>0.39416699999999999</v>
+        <v>12542.7</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>1.8108716525702104</v>
+        <v>0.18331641845841573</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -5468,20 +5364,20 @@
         <v>4096</v>
       </c>
       <c r="B33">
-        <v>1.1657090000000001</v>
+        <v>104733.46</v>
       </c>
       <c r="D33">
-        <v>0.93962500000000004</v>
+        <v>152643.62</v>
       </c>
       <c r="F33">
-        <v>0.41212500000000002</v>
+        <v>34864.21</v>
       </c>
       <c r="H33">
-        <v>0.88304199999999999</v>
+        <v>32513.63</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.93978129572967939</v>
+        <v>0.21300353070767059</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -5489,20 +5385,20 @@
         <v>8192</v>
       </c>
       <c r="B34">
-        <v>6.5979999999999999</v>
+        <v>337165.89</v>
       </c>
       <c r="D34">
-        <v>2.9699580000000001</v>
+        <v>220632.31</v>
       </c>
       <c r="F34">
-        <v>1.238791</v>
+        <v>83174.05</v>
       </c>
       <c r="H34">
-        <v>1.9513750000000001</v>
+        <v>81572.61</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>0.65703791097382525</v>
+        <v>0.36972195958062537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed plots, exponential search and matrix generations
</commit_message>
<xml_diff>
--- a/lab_algo.xlsx
+++ b/lab_algo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaori/IdeaProjects/lab1_pestrikv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47240599-0C41-C847-9DA4-DA0EE3823CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F86FB2A-A6BE-C046-8D74-4EF7B6D8BA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D4F34C4-6F3A-D647-AD59-3E2EE28ECA5C}"/>
   </bookViews>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -285,43 +284,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>23.54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134.35</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298.14</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>706.06</c:v>
+                  <c:v>1544</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1435.81</c:v>
+                  <c:v>2966</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3378.67</c:v>
+                  <c:v>6296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7372.43</c:v>
+                  <c:v>20322</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20446.16</c:v>
+                  <c:v>114817</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37361.300000000003</c:v>
+                  <c:v>352328</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41112.11</c:v>
+                  <c:v>719388</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51791.99</c:v>
+                  <c:v>1405629</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104733.46</c:v>
+                  <c:v>3237251</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>337165.89</c:v>
+                  <c:v>9543580</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,43 +521,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>52.12</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>146.75</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>317.36</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>702.8</c:v>
+                  <c:v>1359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1533.23</c:v>
+                  <c:v>2636</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3631.59</c:v>
+                  <c:v>5549</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8626.2199999999993</c:v>
+                  <c:v>13343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18368.57</c:v>
+                  <c:v>31903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21572.13</c:v>
+                  <c:v>74209</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33467.32</c:v>
+                  <c:v>142564</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>68421.039999999994</c:v>
+                  <c:v>299864</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152643.62</c:v>
+                  <c:v>1335687</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>220632.31</c:v>
+                  <c:v>3762314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,43 +757,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>1418.24</c:v>
+                  <c:v>1524</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2124.1999999999998</c:v>
+                  <c:v>2315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2883.17</c:v>
+                  <c:v>2703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2531.6799999999998</c:v>
+                  <c:v>2966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2912.26</c:v>
+                  <c:v>3209</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3267.42</c:v>
+                  <c:v>3083</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4124.63</c:v>
+                  <c:v>3346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4497.5</c:v>
+                  <c:v>3780</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5731.94</c:v>
+                  <c:v>5433</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12147.97</c:v>
+                  <c:v>8279</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22536.21</c:v>
+                  <c:v>19223</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34864.21</c:v>
+                  <c:v>55247</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83174.05</c:v>
+                  <c:v>86582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -994,43 +993,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>30.12</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.569999999999993</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146.4</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>294.20999999999998</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>451.56</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>411.73</c:v>
+                  <c:v>672</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>733.65</c:v>
+                  <c:v>1365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1557.32</c:v>
+                  <c:v>3632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2619.41</c:v>
+                  <c:v>10982</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4903.16</c:v>
+                  <c:v>35428</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12542.7</c:v>
+                  <c:v>75942</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32513.63</c:v>
+                  <c:v>211272</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>81572.61</c:v>
+                  <c:v>359028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,43 +1543,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>23.54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134.35</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298.14</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>706.06</c:v>
+                  <c:v>1544</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1435.81</c:v>
+                  <c:v>2966</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3378.67</c:v>
+                  <c:v>6296</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7372.43</c:v>
+                  <c:v>20322</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20446.16</c:v>
+                  <c:v>114817</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37361.300000000003</c:v>
+                  <c:v>352328</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41112.11</c:v>
+                  <c:v>719388</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51791.99</c:v>
+                  <c:v>1405629</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104733.46</c:v>
+                  <c:v>3237251</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>337165.89</c:v>
+                  <c:v>9543580</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,43 +1779,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>52.12</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>146.75</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>317.36</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>702.8</c:v>
+                  <c:v>1359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1533.23</c:v>
+                  <c:v>2636</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3631.59</c:v>
+                  <c:v>5549</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8626.2199999999993</c:v>
+                  <c:v>13343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18368.57</c:v>
+                  <c:v>31903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21572.13</c:v>
+                  <c:v>74209</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33467.32</c:v>
+                  <c:v>142564</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>68421.039999999994</c:v>
+                  <c:v>299864</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152643.62</c:v>
+                  <c:v>1335687</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>220632.31</c:v>
+                  <c:v>3762314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,43 +2017,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>1418.24</c:v>
+                  <c:v>1524</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2124.1999999999998</c:v>
+                  <c:v>2315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2883.17</c:v>
+                  <c:v>2703</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2531.6799999999998</c:v>
+                  <c:v>2966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2912.26</c:v>
+                  <c:v>3209</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3267.42</c:v>
+                  <c:v>3083</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4124.63</c:v>
+                  <c:v>3346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4497.5</c:v>
+                  <c:v>3780</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5731.94</c:v>
+                  <c:v>5433</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12147.97</c:v>
+                  <c:v>8279</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22536.21</c:v>
+                  <c:v>19223</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34864.21</c:v>
+                  <c:v>55247</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83174.05</c:v>
+                  <c:v>86582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2254,43 +2253,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>30.12</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.569999999999993</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146.4</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>294.20999999999998</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>451.56</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>411.73</c:v>
+                  <c:v>672</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>733.65</c:v>
+                  <c:v>1365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1557.32</c:v>
+                  <c:v>3632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2619.41</c:v>
+                  <c:v>10982</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4903.16</c:v>
+                  <c:v>35428</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12542.7</c:v>
+                  <c:v>75942</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32513.63</c:v>
+                  <c:v>211272</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>81572.61</c:v>
+                  <c:v>359028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2778,43 +2777,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="1">
-                  <c:v>0.57789716039907912</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.49451448040885854</c:v>
+                  <c:v>0.45405405405405408</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46130577262414924</c:v>
+                  <c:v>0.31075110456553756</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41862549800796811</c:v>
+                  <c:v>0.20676968359087564</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29451549995760584</c:v>
+                  <c:v>0.15705614567526555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11337458248315477</c:v>
+                  <c:v>0.12110290142367994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.5048839468504167E-2</c:v>
+                  <c:v>0.10230083189687476</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.4781776697913883E-2</c:v>
+                  <c:v>0.11384509293796821</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12142565430488318</c:v>
+                  <c:v>0.14798744087644355</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14650590486480541</c:v>
+                  <c:v>0.24850593417693106</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.18331641845841573</c:v>
+                  <c:v>0.25325480884667717</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21300353070767059</c:v>
+                  <c:v>0.15817478196613427</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.36972195958062537</c:v>
+                  <c:v>9.5427441728680812E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5087,8 +5086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF42ADF4-ED66-4146-82D9-75147D1EA78B}">
   <dimension ref="A3:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5133,20 +5132,20 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>23.54</v>
+        <v>119</v>
       </c>
       <c r="D22">
-        <v>52.12</v>
+        <v>160</v>
       </c>
       <c r="F22">
-        <v>1418.24</v>
+        <v>1524</v>
       </c>
       <c r="H22">
-        <v>30.12</v>
+        <v>132</v>
       </c>
       <c r="J22">
         <f t="shared" ref="J22:J34" si="0">(H22/D22)</f>
-        <v>0.57789716039907912</v>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -5154,20 +5153,20 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>134.35</v>
+        <v>410</v>
       </c>
       <c r="D23">
-        <v>146.75</v>
+        <v>370</v>
       </c>
       <c r="F23">
-        <v>2124.1999999999998</v>
+        <v>2315</v>
       </c>
       <c r="H23">
-        <v>72.569999999999993</v>
+        <v>168</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>0.49451448040885854</v>
+        <v>0.45405405405405408</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -5175,20 +5174,20 @@
         <v>8</v>
       </c>
       <c r="B24">
-        <v>298.14</v>
+        <v>750</v>
       </c>
       <c r="D24">
-        <v>317.36</v>
+        <v>679</v>
       </c>
       <c r="F24">
-        <v>2883.17</v>
+        <v>2703</v>
       </c>
       <c r="H24">
-        <v>146.4</v>
+        <v>211</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>0.46130577262414924</v>
+        <v>0.31075110456553756</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -5196,20 +5195,20 @@
         <v>16</v>
       </c>
       <c r="B25">
-        <v>706.06</v>
+        <v>1544</v>
       </c>
       <c r="D25">
-        <v>702.8</v>
+        <v>1359</v>
       </c>
       <c r="F25">
-        <v>2531.6799999999998</v>
+        <v>2966</v>
       </c>
       <c r="H25">
-        <v>294.20999999999998</v>
+        <v>281</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>0.41862549800796811</v>
+        <v>0.20676968359087564</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -5217,20 +5216,20 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>1435.81</v>
+        <v>2966</v>
       </c>
       <c r="D26">
-        <v>1533.23</v>
+        <v>2636</v>
       </c>
       <c r="F26">
-        <v>2912.26</v>
+        <v>3209</v>
       </c>
       <c r="H26">
-        <v>451.56</v>
+        <v>414</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0.29451549995760584</v>
+        <v>0.15705614567526555</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -5238,20 +5237,20 @@
         <v>64</v>
       </c>
       <c r="B27">
-        <v>3378.67</v>
+        <v>6296</v>
       </c>
       <c r="D27">
-        <v>3631.59</v>
+        <v>5549</v>
       </c>
       <c r="F27">
-        <v>3267.42</v>
+        <v>3083</v>
       </c>
       <c r="H27">
-        <v>411.73</v>
+        <v>672</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.11337458248315477</v>
+        <v>0.12110290142367994</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -5259,20 +5258,20 @@
         <v>128</v>
       </c>
       <c r="B28">
-        <v>7372.43</v>
+        <v>20322</v>
       </c>
       <c r="D28">
-        <v>8626.2199999999993</v>
+        <v>13343</v>
       </c>
       <c r="F28">
-        <v>4124.63</v>
+        <v>3346</v>
       </c>
       <c r="H28">
-        <v>733.65</v>
+        <v>1365</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>8.5048839468504167E-2</v>
+        <v>0.10230083189687476</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -5280,20 +5279,20 @@
         <v>256</v>
       </c>
       <c r="B29">
-        <v>20446.16</v>
+        <v>114817</v>
       </c>
       <c r="D29">
-        <v>18368.57</v>
+        <v>31903</v>
       </c>
       <c r="F29">
-        <v>4497.5</v>
+        <v>3780</v>
       </c>
       <c r="H29">
-        <v>1557.32</v>
+        <v>3632</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>8.4781776697913883E-2</v>
+        <v>0.11384509293796821</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -5301,20 +5300,20 @@
         <v>512</v>
       </c>
       <c r="B30">
-        <v>37361.300000000003</v>
+        <v>352328</v>
       </c>
       <c r="D30">
-        <v>21572.13</v>
+        <v>74209</v>
       </c>
       <c r="F30">
-        <v>5731.94</v>
+        <v>5433</v>
       </c>
       <c r="H30">
-        <v>2619.41</v>
+        <v>10982</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0.12142565430488318</v>
+        <v>0.14798744087644355</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -5322,20 +5321,20 @@
         <v>1024</v>
       </c>
       <c r="B31">
-        <v>41112.11</v>
+        <v>719388</v>
       </c>
       <c r="D31">
-        <v>33467.32</v>
+        <v>142564</v>
       </c>
       <c r="F31">
-        <v>12147.97</v>
+        <v>8279</v>
       </c>
       <c r="H31">
-        <v>4903.16</v>
+        <v>35428</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0.14650590486480541</v>
+        <v>0.24850593417693106</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -5343,20 +5342,20 @@
         <v>2048</v>
       </c>
       <c r="B32">
-        <v>51791.99</v>
+        <v>1405629</v>
       </c>
       <c r="D32">
-        <v>68421.039999999994</v>
+        <v>299864</v>
       </c>
       <c r="F32">
-        <v>22536.21</v>
+        <v>19223</v>
       </c>
       <c r="H32">
-        <v>12542.7</v>
+        <v>75942</v>
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>0.18331641845841573</v>
+        <v>0.25325480884667717</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -5364,20 +5363,20 @@
         <v>4096</v>
       </c>
       <c r="B33">
-        <v>104733.46</v>
+        <v>3237251</v>
       </c>
       <c r="D33">
-        <v>152643.62</v>
+        <v>1335687</v>
       </c>
       <c r="F33">
-        <v>34864.21</v>
+        <v>55247</v>
       </c>
       <c r="H33">
-        <v>32513.63</v>
+        <v>211272</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>0.21300353070767059</v>
+        <v>0.15817478196613427</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -5385,20 +5384,20 @@
         <v>8192</v>
       </c>
       <c r="B34">
-        <v>337165.89</v>
+        <v>9543580</v>
       </c>
       <c r="D34">
-        <v>220632.31</v>
+        <v>3762314</v>
       </c>
       <c r="F34">
-        <v>83174.05</v>
+        <v>86582</v>
       </c>
       <c r="H34">
-        <v>81572.61</v>
+        <v>359028</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>0.36972195958062537</v>
+        <v>9.5427441728680812E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>